<commit_message>
remove link to rj45 digikey
</commit_message>
<xml_diff>
--- a/Component_Placement_Sheet.xlsx
+++ b/Component_Placement_Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saxani/My Drive/CosmicWatch/GitHub/CosmicWatch-Desktop-Muon-Detector-v3X/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0061E2BA-F152-1A47-A91D-7E20479F5329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502BE373-B7A4-804F-9FD5-5FF756327F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="760" windowWidth="24540" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="206">
   <si>
     <t>1k</t>
   </si>
@@ -942,6 +942,57 @@
     <xf numFmtId="49" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -967,57 +1018,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3072,8 +3072,8 @@
   </sheetPr>
   <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3092,30 +3092,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="38"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="39"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="41"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
@@ -3139,29 +3139,29 @@
       <c r="G3" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="I3" s="32" t="s">
+      <c r="I3" s="25" t="s">
         <v>203</v>
       </c>
-      <c r="J3" s="33"/>
+      <c r="J3" s="26"/>
     </row>
     <row r="4" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="39" t="s">
         <v>148</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="34" t="s">
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="23" t="s">
         <v>204</v>
       </c>
-      <c r="J4" s="34" t="s">
+      <c r="J4" s="23" t="s">
         <v>194</v>
       </c>
     </row>
@@ -3183,11 +3183,11 @@
       <c r="G5" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H5" s="27"/>
-      <c r="I5" s="31">
+      <c r="H5" s="18"/>
+      <c r="I5" s="22">
         <v>0.1</v>
       </c>
-      <c r="J5" s="31">
+      <c r="J5" s="22">
         <v>0.12</v>
       </c>
     </row>
@@ -3209,11 +3209,11 @@
       <c r="G6" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H6" s="28"/>
-      <c r="I6" s="31">
+      <c r="H6" s="19"/>
+      <c r="I6" s="22">
         <v>0.1</v>
       </c>
-      <c r="J6" s="31">
+      <c r="J6" s="22">
         <v>0.25</v>
       </c>
     </row>
@@ -3235,11 +3235,11 @@
       <c r="G7" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H7" s="28"/>
-      <c r="I7" s="31">
+      <c r="H7" s="19"/>
+      <c r="I7" s="22">
         <v>0.1</v>
       </c>
-      <c r="J7" s="31">
+      <c r="J7" s="22">
         <v>0.14000000000000001</v>
       </c>
     </row>
@@ -3261,11 +3261,11 @@
       <c r="G8" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H8" s="28"/>
-      <c r="I8" s="31">
+      <c r="H8" s="19"/>
+      <c r="I8" s="22">
         <v>0.1</v>
       </c>
-      <c r="J8" s="31">
+      <c r="J8" s="22">
         <v>0.25</v>
       </c>
     </row>
@@ -3289,11 +3289,11 @@
       <c r="G9" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H9" s="28"/>
-      <c r="I9" s="31">
+      <c r="H9" s="19"/>
+      <c r="I9" s="22">
         <v>0.1</v>
       </c>
-      <c r="J9" s="31">
+      <c r="J9" s="22">
         <v>0.27</v>
       </c>
     </row>
@@ -3315,11 +3315,11 @@
       <c r="G10" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H10" s="29"/>
-      <c r="I10" s="31">
+      <c r="H10" s="20"/>
+      <c r="I10" s="22">
         <v>0.19</v>
       </c>
-      <c r="J10" s="31">
+      <c r="J10" s="22">
         <v>1.08</v>
       </c>
     </row>
@@ -3341,11 +3341,11 @@
       <c r="G11" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H11" s="29"/>
-      <c r="I11" s="31">
+      <c r="H11" s="20"/>
+      <c r="I11" s="22">
         <v>0.11</v>
       </c>
-      <c r="J11" s="31">
+      <c r="J11" s="22">
         <v>0.63</v>
       </c>
     </row>
@@ -3367,11 +3367,11 @@
       <c r="G12" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H12" s="29"/>
-      <c r="I12" s="31">
+      <c r="H12" s="20"/>
+      <c r="I12" s="22">
         <v>0.08</v>
       </c>
-      <c r="J12" s="31">
+      <c r="J12" s="22">
         <v>0.08</v>
       </c>
     </row>
@@ -3393,11 +3393,11 @@
       <c r="G13" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H13" s="29"/>
-      <c r="I13" s="31">
+      <c r="H13" s="20"/>
+      <c r="I13" s="22">
         <v>0.1</v>
       </c>
-      <c r="J13" s="31">
+      <c r="J13" s="22">
         <v>0.22</v>
       </c>
     </row>
@@ -3421,11 +3421,11 @@
       <c r="G14" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H14" s="29"/>
-      <c r="I14" s="31">
+      <c r="H14" s="20"/>
+      <c r="I14" s="22">
         <v>1.04</v>
       </c>
-      <c r="J14" s="31">
+      <c r="J14" s="22">
         <v>6.31</v>
       </c>
     </row>
@@ -3449,27 +3449,27 @@
       <c r="G15" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H15" s="29"/>
-      <c r="I15" s="31">
+      <c r="H15" s="20"/>
+      <c r="I15" s="22">
         <v>4</v>
       </c>
-      <c r="J15" s="31">
+      <c r="J15" s="22">
         <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="43" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="10">
@@ -3489,11 +3489,11 @@
       <c r="G17" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H17" s="29"/>
-      <c r="I17" s="31">
+      <c r="H17" s="20"/>
+      <c r="I17" s="22">
         <v>0.15</v>
       </c>
-      <c r="J17" s="31">
+      <c r="J17" s="22">
         <v>1.22</v>
       </c>
     </row>
@@ -3515,11 +3515,11 @@
       <c r="G18" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H18" s="29"/>
-      <c r="I18" s="31">
+      <c r="H18" s="20"/>
+      <c r="I18" s="22">
         <v>0.1</v>
       </c>
-      <c r="J18" s="31">
+      <c r="J18" s="22">
         <v>0.54</v>
       </c>
     </row>
@@ -3543,11 +3543,11 @@
       <c r="G19" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H19" s="29"/>
-      <c r="I19" s="31">
+      <c r="H19" s="20"/>
+      <c r="I19" s="22">
         <v>1.92</v>
       </c>
-      <c r="J19" s="31">
+      <c r="J19" s="22">
         <v>11.92</v>
       </c>
     </row>
@@ -3571,11 +3571,11 @@
       <c r="G20" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H20" s="29"/>
-      <c r="I20" s="31">
+      <c r="H20" s="20"/>
+      <c r="I20" s="22">
         <v>1.67</v>
       </c>
-      <c r="J20" s="31">
+      <c r="J20" s="22">
         <v>12.26</v>
       </c>
     </row>
@@ -3599,11 +3599,11 @@
       <c r="G21" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H21" s="29"/>
-      <c r="I21" s="31">
+      <c r="H21" s="20"/>
+      <c r="I21" s="22">
         <v>0.14000000000000001</v>
       </c>
-      <c r="J21" s="31">
+      <c r="J21" s="22">
         <v>1.08</v>
       </c>
     </row>
@@ -3627,11 +3627,11 @@
       <c r="G22" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H22" s="29"/>
-      <c r="I22" s="31">
+      <c r="H22" s="20"/>
+      <c r="I22" s="22">
         <v>0.1</v>
       </c>
-      <c r="J22" s="31">
+      <c r="J22" s="22">
         <v>0.61</v>
       </c>
     </row>
@@ -3655,11 +3655,11 @@
       <c r="G23" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H23" s="29"/>
-      <c r="I23" s="31">
+      <c r="H23" s="20"/>
+      <c r="I23" s="22">
         <v>0.13</v>
       </c>
-      <c r="J23" s="31">
+      <c r="J23" s="22">
         <v>0.8</v>
       </c>
     </row>
@@ -3683,27 +3683,27 @@
       <c r="G24" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H24" s="29"/>
-      <c r="I24" s="31">
+      <c r="H24" s="20"/>
+      <c r="I24" s="22">
         <v>0.89</v>
       </c>
-      <c r="J24" s="31">
+      <c r="J24" s="22">
         <v>7.55</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="41" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="33" t="s">
         <v>187</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
     </row>
     <row r="26" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="10">
@@ -3723,11 +3723,11 @@
       <c r="G26" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H26" s="29"/>
-      <c r="I26" s="31">
+      <c r="H26" s="20"/>
+      <c r="I26" s="22">
         <v>0.1</v>
       </c>
-      <c r="J26" s="31">
+      <c r="J26" s="22">
         <v>0.14000000000000001</v>
       </c>
     </row>
@@ -3749,11 +3749,11 @@
       <c r="G27" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H27" s="29"/>
-      <c r="I27" s="31">
+      <c r="H27" s="20"/>
+      <c r="I27" s="22">
         <v>0.1</v>
       </c>
-      <c r="J27" s="31">
+      <c r="J27" s="22">
         <v>0.12</v>
       </c>
     </row>
@@ -3775,11 +3775,11 @@
       <c r="G28" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H28" s="29"/>
-      <c r="I28" s="31">
+      <c r="H28" s="20"/>
+      <c r="I28" s="22">
         <v>0.1</v>
       </c>
-      <c r="J28" s="31">
+      <c r="J28" s="22">
         <v>0.12</v>
       </c>
     </row>
@@ -3801,11 +3801,11 @@
       <c r="G29" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H29" s="29"/>
-      <c r="I29" s="31">
+      <c r="H29" s="20"/>
+      <c r="I29" s="22">
         <v>0.13</v>
       </c>
-      <c r="J29" s="31">
+      <c r="J29" s="22">
         <v>0.16</v>
       </c>
     </row>
@@ -3827,11 +3827,11 @@
       <c r="G30" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H30" s="29"/>
-      <c r="I30" s="31">
+      <c r="H30" s="20"/>
+      <c r="I30" s="22">
         <v>0.1</v>
       </c>
-      <c r="J30" s="31">
+      <c r="J30" s="22">
         <v>0.49</v>
       </c>
     </row>
@@ -3855,11 +3855,11 @@
       <c r="G31" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H31" s="29"/>
-      <c r="I31" s="31">
+      <c r="H31" s="20"/>
+      <c r="I31" s="22">
         <v>0.13</v>
       </c>
-      <c r="J31" s="31">
+      <c r="J31" s="22">
         <v>0.73</v>
       </c>
     </row>
@@ -3883,29 +3883,29 @@
       <c r="G32" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H32" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="I32" s="31">
+      <c r="H32" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="I32" s="22">
         <v>2.48</v>
       </c>
-      <c r="J32" s="31">
+      <c r="J32" s="22">
         <v>21.07</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
     </row>
     <row r="34" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="10">
@@ -3927,13 +3927,13 @@
       <c r="G34" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H34" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="I34" s="31">
+      <c r="H34" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="I34" s="22">
         <v>0.33</v>
       </c>
-      <c r="J34" s="31">
+      <c r="J34" s="22">
         <v>2.82</v>
       </c>
     </row>
@@ -3954,16 +3954,14 @@
       <c r="F35" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="G35" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="H35" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="I35" s="31">
+      <c r="G35" s="4"/>
+      <c r="H35" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="I35" s="22">
         <v>0.45</v>
       </c>
-      <c r="J35" s="31">
+      <c r="J35" s="22">
         <v>3.83</v>
       </c>
     </row>
@@ -3987,14 +3985,14 @@
       <c r="G36" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H36" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="I36" s="35">
+      <c r="H36" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="I36" s="24">
         <f>6.89/10</f>
         <v>0.68899999999999995</v>
       </c>
-      <c r="J36" s="31">
+      <c r="J36" s="22">
         <v>6.89</v>
       </c>
     </row>
@@ -4018,14 +4016,14 @@
       <c r="G37" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H37" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="I37" s="31">
+      <c r="H37" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="I37" s="22">
         <f>7.39/5</f>
         <v>1.478</v>
       </c>
-      <c r="J37" s="31">
+      <c r="J37" s="22">
         <f>7.39*2</f>
         <v>14.78</v>
       </c>
@@ -4050,11 +4048,11 @@
       <c r="G38" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H38" s="29"/>
-      <c r="I38" s="31">
+      <c r="H38" s="20"/>
+      <c r="I38" s="22">
         <v>6.99</v>
       </c>
-      <c r="J38" s="31">
+      <c r="J38" s="22">
         <f>3.663333333*10</f>
         <v>36.633333329999999</v>
       </c>
@@ -4079,12 +4077,12 @@
       <c r="G39" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H39" s="29"/>
-      <c r="I39" s="35">
+      <c r="H39" s="20"/>
+      <c r="I39" s="24">
         <f>6.99/100</f>
         <v>6.9900000000000004E-2</v>
       </c>
-      <c r="J39" s="31">
+      <c r="J39" s="22">
         <f>6.99/10</f>
         <v>0.69900000000000007</v>
       </c>
@@ -4109,12 +4107,12 @@
       <c r="G40" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H40" s="29"/>
-      <c r="I40" s="31">
+      <c r="H40" s="20"/>
+      <c r="I40" s="22">
         <f>6.99/100</f>
         <v>6.9900000000000004E-2</v>
       </c>
-      <c r="J40" s="31">
+      <c r="J40" s="22">
         <f>6.99/10</f>
         <v>0.69900000000000007</v>
       </c>
@@ -4139,13 +4137,13 @@
       <c r="G41" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H41" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="I41" s="31">
+      <c r="H41" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="I41" s="22">
         <v>5</v>
       </c>
-      <c r="J41" s="31">
+      <c r="J41" s="22">
         <v>28</v>
       </c>
     </row>
@@ -4169,31 +4167,31 @@
       <c r="G42" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H42" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="I42" s="31">
+      <c r="H42" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="I42" s="22">
         <f>7.29/6</f>
         <v>1.2150000000000001</v>
       </c>
-      <c r="J42" s="31">
+      <c r="J42" s="22">
         <f>I42*10</f>
         <v>12.15</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="16" t="s">
+      <c r="A43" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="B43" s="17"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="31"/>
-      <c r="J43" s="31"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="34"/>
+      <c r="G43" s="35"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="14">
@@ -4213,11 +4211,11 @@
       <c r="G44" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H44" s="29"/>
-      <c r="I44" s="31">
+      <c r="H44" s="20"/>
+      <c r="I44" s="22">
         <v>0.11</v>
       </c>
-      <c r="J44" s="31">
+      <c r="J44" s="22">
         <v>0.61</v>
       </c>
     </row>
@@ -4239,11 +4237,11 @@
       <c r="G45" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H45" s="29"/>
-      <c r="I45" s="31">
+      <c r="H45" s="20"/>
+      <c r="I45" s="22">
         <v>0.08</v>
       </c>
-      <c r="J45" s="31">
+      <c r="J45" s="22">
         <v>0.11</v>
       </c>
     </row>
@@ -4265,11 +4263,11 @@
       <c r="G46" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H46" s="29"/>
-      <c r="I46" s="31">
+      <c r="H46" s="20"/>
+      <c r="I46" s="22">
         <v>0.08</v>
       </c>
-      <c r="J46" s="31">
+      <c r="J46" s="22">
         <v>0.08</v>
       </c>
     </row>
@@ -4291,11 +4289,11 @@
       <c r="G47" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H47" s="29"/>
-      <c r="I47" s="31">
+      <c r="H47" s="20"/>
+      <c r="I47" s="22">
         <v>0.11</v>
       </c>
-      <c r="J47" s="31">
+      <c r="J47" s="22">
         <v>0.35</v>
       </c>
     </row>
@@ -4317,11 +4315,11 @@
       <c r="G48" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H48" s="29"/>
-      <c r="I48" s="31">
+      <c r="H48" s="20"/>
+      <c r="I48" s="22">
         <v>0.1</v>
       </c>
-      <c r="J48" s="31">
+      <c r="J48" s="22">
         <v>0.25</v>
       </c>
     </row>
@@ -4345,11 +4343,11 @@
       <c r="G49" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H49" s="29"/>
-      <c r="I49" s="31">
+      <c r="H49" s="20"/>
+      <c r="I49" s="22">
         <v>0.53</v>
       </c>
-      <c r="J49" s="31">
+      <c r="J49" s="22">
         <v>4.51</v>
       </c>
     </row>
@@ -4373,11 +4371,11 @@
       <c r="G50" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H50" s="29"/>
-      <c r="I50" s="31">
+      <c r="H50" s="20"/>
+      <c r="I50" s="22">
         <v>28.41</v>
       </c>
-      <c r="J50" s="31">
+      <c r="J50" s="22">
         <v>251.47</v>
       </c>
     </row>
@@ -4401,11 +4399,11 @@
       <c r="G51" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H51" s="29"/>
-      <c r="I51" s="31">
+      <c r="H51" s="20"/>
+      <c r="I51" s="22">
         <v>0.7</v>
       </c>
-      <c r="J51" s="31">
+      <c r="J51" s="22">
         <v>5.9</v>
       </c>
     </row>
@@ -4429,29 +4427,29 @@
       <c r="G52" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H52" s="29"/>
-      <c r="I52" s="31">
+      <c r="H52" s="20"/>
+      <c r="I52" s="22">
         <f>6.79/100</f>
         <v>6.7900000000000002E-2</v>
       </c>
-      <c r="J52" s="31">
+      <c r="J52" s="22">
         <f>6.79/10</f>
         <v>0.67900000000000005</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="19" t="s">
+      <c r="A53" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="21"/>
-      <c r="H53" s="21"/>
-      <c r="I53" s="31"/>
-      <c r="J53" s="31"/>
+      <c r="B53" s="37"/>
+      <c r="C53" s="37"/>
+      <c r="D53" s="37"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="37"/>
+      <c r="G53" s="38"/>
+      <c r="H53" s="38"/>
+      <c r="I53" s="22"/>
+      <c r="J53" s="22"/>
     </row>
     <row r="54" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="14">
@@ -4471,11 +4469,11 @@
       <c r="G54" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H54" s="29"/>
-      <c r="I54" s="31">
+      <c r="H54" s="20"/>
+      <c r="I54" s="22">
         <v>19</v>
       </c>
-      <c r="J54" s="31">
+      <c r="J54" s="22">
         <v>190</v>
       </c>
     </row>
@@ -4499,11 +4497,11 @@
       <c r="G55" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H55" s="29"/>
-      <c r="I55" s="31">
+      <c r="H55" s="20"/>
+      <c r="I55" s="22">
         <v>0.1</v>
       </c>
-      <c r="J55" s="31">
+      <c r="J55" s="22">
         <v>0.1</v>
       </c>
     </row>
@@ -4525,11 +4523,11 @@
       <c r="G56" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H56" s="30"/>
-      <c r="I56" s="31">
+      <c r="H56" s="21"/>
+      <c r="I56" s="22">
         <v>9.9499999999999993</v>
       </c>
-      <c r="J56" s="31">
+      <c r="J56" s="22">
         <v>9.9499999999999993</v>
       </c>
     </row>
@@ -4553,12 +4551,12 @@
       <c r="G57" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H57" s="29"/>
-      <c r="I57" s="35">
+      <c r="H57" s="20"/>
+      <c r="I57" s="24">
         <f>12.69/10</f>
         <v>1.2689999999999999</v>
       </c>
-      <c r="J57" s="31">
+      <c r="J57" s="22">
         <v>12.69</v>
       </c>
     </row>
@@ -4582,12 +4580,12 @@
       <c r="G58" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H58" s="29"/>
-      <c r="I58" s="35">
+      <c r="H58" s="20"/>
+      <c r="I58" s="24">
         <f>2.65/100</f>
         <v>2.6499999999999999E-2</v>
       </c>
-      <c r="J58" s="31">
+      <c r="J58" s="22">
         <f>I58*10</f>
         <v>0.26500000000000001</v>
       </c>
@@ -4612,11 +4610,11 @@
       <c r="G59" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H59" s="29"/>
-      <c r="I59" s="31">
+      <c r="H59" s="20"/>
+      <c r="I59" s="22">
         <v>1.69</v>
       </c>
-      <c r="J59" s="31">
+      <c r="J59" s="22">
         <v>16.920000000000002</v>
       </c>
     </row>
@@ -4640,14 +4638,14 @@
       <c r="G60" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H60" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="I60" s="35">
+      <c r="H60" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="I60" s="24">
         <f>8.89/6</f>
         <v>1.4816666666666667</v>
       </c>
-      <c r="J60" s="31">
+      <c r="J60" s="22">
         <f>8.89</f>
         <v>8.89</v>
       </c>
@@ -4672,11 +4670,11 @@
       <c r="G61" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H61" s="30"/>
-      <c r="I61" s="31">
+      <c r="H61" s="21"/>
+      <c r="I61" s="22">
         <v>9</v>
       </c>
-      <c r="J61" s="31">
+      <c r="J61" s="22">
         <v>90</v>
       </c>
     </row>
@@ -4698,14 +4696,14 @@
       <c r="G62" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H62" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="I62" s="35">
+      <c r="H62" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="I62" s="24">
         <f>3.99/100</f>
         <v>3.9900000000000005E-2</v>
       </c>
-      <c r="J62" s="31">
+      <c r="J62" s="22">
         <f>100*I62</f>
         <v>3.9900000000000007</v>
       </c>
@@ -4728,14 +4726,14 @@
       <c r="G63" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H63" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="I63" s="31">
+      <c r="H63" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="I63" s="22">
         <f>6.09/20</f>
         <v>0.30449999999999999</v>
       </c>
-      <c r="J63" s="31">
+      <c r="J63" s="22">
         <f>I63*10</f>
         <v>3.0449999999999999</v>
       </c>
@@ -4758,14 +4756,14 @@
       <c r="G64" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H64" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="I64" s="31">
+      <c r="H64" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="I64" s="22">
         <f>11.39/100</f>
         <v>0.1139</v>
       </c>
-      <c r="J64" s="31">
+      <c r="J64" s="22">
         <f>I64*10</f>
         <v>1.139</v>
       </c>
@@ -4790,11 +4788,11 @@
       <c r="G65" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H65" s="30"/>
-      <c r="I65" s="31">
+      <c r="H65" s="21"/>
+      <c r="I65" s="22">
         <v>1</v>
       </c>
-      <c r="J65" s="31">
+      <c r="J65" s="22">
         <v>5</v>
       </c>
     </row>
@@ -4816,13 +4814,13 @@
       <c r="G66" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H66" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="I66" s="31">
+      <c r="H66" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="I66" s="22">
         <v>7.19</v>
       </c>
-      <c r="J66" s="31">
+      <c r="J66" s="22">
         <v>7.19</v>
       </c>
     </row>
@@ -4844,24 +4842,24 @@
       <c r="G67" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H67" s="27"/>
-      <c r="I67" s="31">
+      <c r="H67" s="18"/>
+      <c r="I67" s="22">
         <v>2.5</v>
       </c>
-      <c r="J67" s="31">
+      <c r="J67" s="22">
         <v>25</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="G68" s="25" t="s">
+      <c r="G68" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="H68" s="25"/>
-      <c r="I68" s="25">
+      <c r="H68" s="16"/>
+      <c r="I68" s="16">
         <f>SUM(I5:I67)</f>
         <v>114.40516666666667</v>
       </c>
-      <c r="J68" s="25">
+      <c r="J68" s="16">
         <f>SUM(J5:J67)</f>
         <v>852.79933333000008</v>
       </c>
@@ -4904,56 +4902,55 @@
     <hyperlink ref="G31" r:id="rId24" xr:uid="{92EA5DFD-5C62-C249-A4BA-C8D51F259335}"/>
     <hyperlink ref="G32" r:id="rId25" xr:uid="{DAA65368-96A4-F649-80C6-47C27D6E77EB}"/>
     <hyperlink ref="G34" r:id="rId26" xr:uid="{BCFBE50A-4F43-E041-A2B0-3A39ACB29628}"/>
-    <hyperlink ref="G35" r:id="rId27" xr:uid="{F3140CEC-2E75-F04D-8FD5-ED1DA7AC1A9F}"/>
-    <hyperlink ref="G36" r:id="rId28" xr:uid="{28B79E98-1696-BE46-87D2-E047D9390A4B}"/>
-    <hyperlink ref="G38" r:id="rId29" xr:uid="{060B0E4E-853A-4744-8793-0FB142CBAFA5}"/>
-    <hyperlink ref="G39" r:id="rId30" xr:uid="{704EA759-3F24-1E43-9225-F3EF4AF1D8AE}"/>
-    <hyperlink ref="G40" r:id="rId31" xr:uid="{51DEB24F-F2D8-034B-B4CE-B862AFD8AEF4}"/>
-    <hyperlink ref="G42" r:id="rId32" xr:uid="{2699EBE7-D782-624D-89C6-8E001041169F}"/>
-    <hyperlink ref="G44" r:id="rId33" xr:uid="{627C4F45-41F7-F540-B4E2-2728848CDE60}"/>
-    <hyperlink ref="G51" r:id="rId34" xr:uid="{4D237FA4-6FE9-5A4C-8713-4FCD965F5231}"/>
-    <hyperlink ref="G52" r:id="rId35" xr:uid="{4E031D5E-4B15-E646-AA8E-47A65B6EFF79}"/>
-    <hyperlink ref="G62" r:id="rId36" xr:uid="{FDE7FB9D-D7E4-7544-96B1-C85422C1CAA7}"/>
-    <hyperlink ref="G61" r:id="rId37" xr:uid="{6AE9298E-B5B2-DD44-8E1C-0E89BF893AE6}"/>
-    <hyperlink ref="G59" r:id="rId38" xr:uid="{7F05D5E5-E6BA-CD40-BF00-3E6A222ACF58}"/>
-    <hyperlink ref="G55" r:id="rId39" xr:uid="{81004994-FC78-8547-9153-583C44AE1D76}"/>
-    <hyperlink ref="G58" r:id="rId40" xr:uid="{A7A3D3E7-DB98-9846-9837-4F92A5AEC05B}"/>
-    <hyperlink ref="G63" r:id="rId41" xr:uid="{A4C11252-F340-8C41-94EA-7F54CBE97C72}"/>
-    <hyperlink ref="G64" r:id="rId42" xr:uid="{9754C7AB-196A-6549-BEAD-D36381163F48}"/>
-    <hyperlink ref="G67" r:id="rId43" xr:uid="{4398D883-8521-194B-8F9B-83CB9FAC708C}"/>
-    <hyperlink ref="G60" r:id="rId44" xr:uid="{8121FC13-B5AD-DE45-B596-7A654553B8E1}"/>
-    <hyperlink ref="G56" r:id="rId45" xr:uid="{5239B69E-6ECC-9A44-AB79-B03D6976AB4B}"/>
-    <hyperlink ref="G65" r:id="rId46" xr:uid="{2649F7DB-4C28-0842-86F0-046A8CBD0D7F}"/>
-    <hyperlink ref="G57" r:id="rId47" xr:uid="{8E7EBB42-4FF3-2040-B177-E71E2A9B513B}"/>
-    <hyperlink ref="G9" r:id="rId48" xr:uid="{4D3355E8-5A36-174A-A71D-DB31B3BDB127}"/>
-    <hyperlink ref="G37" r:id="rId49" xr:uid="{565D2868-B2F4-4147-8B2C-9DA2839B402A}"/>
-    <hyperlink ref="G6" r:id="rId50" xr:uid="{41337B6D-A726-404F-8E3A-A7297AAEF553}"/>
-    <hyperlink ref="G45" r:id="rId51" xr:uid="{34D85EC0-0AEE-374A-B6A1-76DF8A07B165}"/>
-    <hyperlink ref="G46" r:id="rId52" xr:uid="{EDB9A295-1581-C24A-88A3-E0CC212C0DDD}"/>
-    <hyperlink ref="G47" r:id="rId53" xr:uid="{6DE2C368-613C-9D4D-9F84-6D0DBC951923}"/>
-    <hyperlink ref="G48" r:id="rId54" xr:uid="{4DC302ED-59A9-2449-A361-F29906F9C3AE}"/>
-    <hyperlink ref="H32" r:id="rId55" xr:uid="{D70B5C5F-26F0-0B41-8C17-1CC14ADA3FE6}"/>
-    <hyperlink ref="H34" r:id="rId56" xr:uid="{0641F1EB-124F-B04D-A94A-758F384DED86}"/>
-    <hyperlink ref="H35" r:id="rId57" xr:uid="{DB0D0FF9-650C-9047-8B87-64100B2B793F}"/>
-    <hyperlink ref="H36" r:id="rId58" xr:uid="{C2D15776-74B0-F248-A49B-2B60EC4E9F50}"/>
-    <hyperlink ref="H37" r:id="rId59" xr:uid="{7FCBF6EC-A974-3C4D-8ECC-BADD5D52FD8F}"/>
-    <hyperlink ref="H41" r:id="rId60" xr:uid="{FF2327CA-6C12-1B4D-9F3D-A6892FDF93AA}"/>
-    <hyperlink ref="G41" r:id="rId61" xr:uid="{A3991D56-3C5A-D24F-9BF4-72B691163E2E}"/>
-    <hyperlink ref="H42" r:id="rId62" xr:uid="{85C3CCAE-AE34-6F4D-BB81-D0542993FD86}"/>
-    <hyperlink ref="G50" r:id="rId63" xr:uid="{6D279AE6-1632-D949-AF1B-D9B01BEE22D5}"/>
-    <hyperlink ref="G54" r:id="rId64" xr:uid="{77ED00C2-AEB9-AF46-BAD4-47C057542ED7}"/>
-    <hyperlink ref="H60" r:id="rId65" xr:uid="{7E92FC71-1828-1347-8A0C-006F6C8E33D9}"/>
-    <hyperlink ref="H62" r:id="rId66" xr:uid="{765DA2F2-534C-F04A-83EE-6DE4C93A616F}"/>
-    <hyperlink ref="H63" r:id="rId67" xr:uid="{2FF58D32-1303-3741-8980-398B83460ED3}"/>
-    <hyperlink ref="H64" r:id="rId68" xr:uid="{26EDE05F-D1A0-2C4A-8936-BE0E610D5348}"/>
-    <hyperlink ref="G66" r:id="rId69" xr:uid="{1F44837E-6CDE-1F4D-ADC9-348EB68867C4}"/>
-    <hyperlink ref="H66" r:id="rId70" xr:uid="{A9E4EEEA-BAD5-8044-925B-73291B6B46E9}"/>
+    <hyperlink ref="G36" r:id="rId27" xr:uid="{28B79E98-1696-BE46-87D2-E047D9390A4B}"/>
+    <hyperlink ref="G38" r:id="rId28" xr:uid="{060B0E4E-853A-4744-8793-0FB142CBAFA5}"/>
+    <hyperlink ref="G39" r:id="rId29" xr:uid="{704EA759-3F24-1E43-9225-F3EF4AF1D8AE}"/>
+    <hyperlink ref="G40" r:id="rId30" xr:uid="{51DEB24F-F2D8-034B-B4CE-B862AFD8AEF4}"/>
+    <hyperlink ref="G42" r:id="rId31" xr:uid="{2699EBE7-D782-624D-89C6-8E001041169F}"/>
+    <hyperlink ref="G44" r:id="rId32" xr:uid="{627C4F45-41F7-F540-B4E2-2728848CDE60}"/>
+    <hyperlink ref="G51" r:id="rId33" xr:uid="{4D237FA4-6FE9-5A4C-8713-4FCD965F5231}"/>
+    <hyperlink ref="G52" r:id="rId34" xr:uid="{4E031D5E-4B15-E646-AA8E-47A65B6EFF79}"/>
+    <hyperlink ref="G62" r:id="rId35" xr:uid="{FDE7FB9D-D7E4-7544-96B1-C85422C1CAA7}"/>
+    <hyperlink ref="G61" r:id="rId36" xr:uid="{6AE9298E-B5B2-DD44-8E1C-0E89BF893AE6}"/>
+    <hyperlink ref="G59" r:id="rId37" xr:uid="{7F05D5E5-E6BA-CD40-BF00-3E6A222ACF58}"/>
+    <hyperlink ref="G55" r:id="rId38" xr:uid="{81004994-FC78-8547-9153-583C44AE1D76}"/>
+    <hyperlink ref="G58" r:id="rId39" xr:uid="{A7A3D3E7-DB98-9846-9837-4F92A5AEC05B}"/>
+    <hyperlink ref="G63" r:id="rId40" xr:uid="{A4C11252-F340-8C41-94EA-7F54CBE97C72}"/>
+    <hyperlink ref="G64" r:id="rId41" xr:uid="{9754C7AB-196A-6549-BEAD-D36381163F48}"/>
+    <hyperlink ref="G67" r:id="rId42" xr:uid="{4398D883-8521-194B-8F9B-83CB9FAC708C}"/>
+    <hyperlink ref="G60" r:id="rId43" xr:uid="{8121FC13-B5AD-DE45-B596-7A654553B8E1}"/>
+    <hyperlink ref="G56" r:id="rId44" xr:uid="{5239B69E-6ECC-9A44-AB79-B03D6976AB4B}"/>
+    <hyperlink ref="G65" r:id="rId45" xr:uid="{2649F7DB-4C28-0842-86F0-046A8CBD0D7F}"/>
+    <hyperlink ref="G57" r:id="rId46" xr:uid="{8E7EBB42-4FF3-2040-B177-E71E2A9B513B}"/>
+    <hyperlink ref="G9" r:id="rId47" xr:uid="{4D3355E8-5A36-174A-A71D-DB31B3BDB127}"/>
+    <hyperlink ref="G37" r:id="rId48" xr:uid="{565D2868-B2F4-4147-8B2C-9DA2839B402A}"/>
+    <hyperlink ref="G6" r:id="rId49" xr:uid="{41337B6D-A726-404F-8E3A-A7297AAEF553}"/>
+    <hyperlink ref="G45" r:id="rId50" xr:uid="{34D85EC0-0AEE-374A-B6A1-76DF8A07B165}"/>
+    <hyperlink ref="G46" r:id="rId51" xr:uid="{EDB9A295-1581-C24A-88A3-E0CC212C0DDD}"/>
+    <hyperlink ref="G47" r:id="rId52" xr:uid="{6DE2C368-613C-9D4D-9F84-6D0DBC951923}"/>
+    <hyperlink ref="G48" r:id="rId53" xr:uid="{4DC302ED-59A9-2449-A361-F29906F9C3AE}"/>
+    <hyperlink ref="H32" r:id="rId54" xr:uid="{D70B5C5F-26F0-0B41-8C17-1CC14ADA3FE6}"/>
+    <hyperlink ref="H34" r:id="rId55" xr:uid="{0641F1EB-124F-B04D-A94A-758F384DED86}"/>
+    <hyperlink ref="H35" r:id="rId56" xr:uid="{DB0D0FF9-650C-9047-8B87-64100B2B793F}"/>
+    <hyperlink ref="H36" r:id="rId57" xr:uid="{C2D15776-74B0-F248-A49B-2B60EC4E9F50}"/>
+    <hyperlink ref="H37" r:id="rId58" xr:uid="{7FCBF6EC-A974-3C4D-8ECC-BADD5D52FD8F}"/>
+    <hyperlink ref="H41" r:id="rId59" xr:uid="{FF2327CA-6C12-1B4D-9F3D-A6892FDF93AA}"/>
+    <hyperlink ref="G41" r:id="rId60" xr:uid="{A3991D56-3C5A-D24F-9BF4-72B691163E2E}"/>
+    <hyperlink ref="H42" r:id="rId61" xr:uid="{85C3CCAE-AE34-6F4D-BB81-D0542993FD86}"/>
+    <hyperlink ref="G50" r:id="rId62" xr:uid="{6D279AE6-1632-D949-AF1B-D9B01BEE22D5}"/>
+    <hyperlink ref="G54" r:id="rId63" xr:uid="{77ED00C2-AEB9-AF46-BAD4-47C057542ED7}"/>
+    <hyperlink ref="H60" r:id="rId64" xr:uid="{7E92FC71-1828-1347-8A0C-006F6C8E33D9}"/>
+    <hyperlink ref="H62" r:id="rId65" xr:uid="{765DA2F2-534C-F04A-83EE-6DE4C93A616F}"/>
+    <hyperlink ref="H63" r:id="rId66" xr:uid="{2FF58D32-1303-3741-8980-398B83460ED3}"/>
+    <hyperlink ref="H64" r:id="rId67" xr:uid="{26EDE05F-D1A0-2C4A-8936-BE0E610D5348}"/>
+    <hyperlink ref="G66" r:id="rId68" xr:uid="{1F44837E-6CDE-1F4D-ADC9-348EB68867C4}"/>
+    <hyperlink ref="H66" r:id="rId69" xr:uid="{A9E4EEEA-BAD5-8044-925B-73291B6B46E9}"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup scale="40" fitToHeight="4" orientation="portrait" copies="2"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId71"/>
+  <drawing r:id="rId70"/>
 </worksheet>
 </file>
</xml_diff>